<commit_message>
update tracking number DC S013
</commit_message>
<xml_diff>
--- a/resourses/testdata/excel_file/Tracking_number.xlsx
+++ b/resourses/testdata/excel_file/Tracking_number.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AU528"/>
+  <dimension ref="A1:AU526"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18:Y241"/>
@@ -728,7 +728,7 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016804</t>
+          <t>SPBD241100016810</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016806</t>
+          <t>SPBD241100016814</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016810</t>
+          <t>SPBD241100016820</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016814</t>
+          <t>SPBD241100016821</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016820</t>
+          <t>SPBD241100016829</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016821</t>
+          <t>SPBD241100016830</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -1622,7 +1622,7 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016829</t>
+          <t>SPBD241100016832</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="B10" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016830</t>
+          <t>SPBD241100016795</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -1920,7 +1920,7 @@
       </c>
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016832</t>
+          <t>SPBD241100016798</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -2069,7 +2069,7 @@
       </c>
       <c r="B12" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016795</t>
+          <t>SPBD241100016807</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -2218,7 +2218,7 @@
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016798</t>
+          <t>SPBD241100016813</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -2367,7 +2367,7 @@
       </c>
       <c r="B14" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016807</t>
+          <t>SPBD241100016815</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -2516,7 +2516,7 @@
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016813</t>
+          <t>SPBD241100016817</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016815</t>
+          <t>SPBD241100016823</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -2814,7 +2814,7 @@
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016817</t>
+          <t>SPBD241100016825</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="B18" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016823</t>
+          <t>SPBD241100016826</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -3112,7 +3112,7 @@
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016825</t>
+          <t>SPBD241100016827</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -3261,7 +3261,7 @@
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016826</t>
+          <t>SPBD241100016834</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -3405,12 +3405,12 @@
     <row r="21" ht="13.2" customHeight="1" thickBot="1">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>20-11-2567</t>
+          <t>21-11-2567</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016827</t>
+          <t>SPBD241100017224</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -3554,12 +3554,12 @@
     <row r="22" ht="13.2" customHeight="1" thickBot="1">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>20-11-2567</t>
+          <t>21-11-2567</t>
         </is>
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100016834</t>
+          <t>SPBD241100017225</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -3708,7 +3708,7 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017224</t>
+          <t>SPBD241100017236</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -3857,7 +3857,7 @@
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017225</t>
+          <t>SPBD241100017242</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
@@ -4006,7 +4006,7 @@
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017236</t>
+          <t>SPBD241100017245</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -4155,7 +4155,7 @@
       </c>
       <c r="B26" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017242</t>
+          <t>SPBD241100017222</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -4304,7 +4304,7 @@
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017245</t>
+          <t>SPBD241100017228</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
@@ -4453,7 +4453,7 @@
       </c>
       <c r="B28" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017222</t>
+          <t>SPBD241100017233</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
@@ -4602,7 +4602,7 @@
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017228</t>
+          <t>SPBD241100017237</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -4751,7 +4751,7 @@
       </c>
       <c r="B30" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017233</t>
+          <t>SPBD241100017248</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -4900,7 +4900,7 @@
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017237</t>
+          <t>SPBD241100017215</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
@@ -5049,7 +5049,7 @@
       </c>
       <c r="B32" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017248</t>
+          <t>SPBD241100017217</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -5198,7 +5198,7 @@
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017215</t>
+          <t>SPBD241100017218</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
@@ -5347,7 +5347,7 @@
       </c>
       <c r="B34" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017217</t>
+          <t>SPBD241100017219</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -5496,7 +5496,7 @@
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017218</t>
+          <t>SPBD241100017226</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
@@ -5645,7 +5645,7 @@
       </c>
       <c r="B36" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017219</t>
+          <t>SPBD241100017232</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
@@ -5794,7 +5794,7 @@
       </c>
       <c r="B37" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017226</t>
+          <t>SPBD241100017235</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
@@ -5943,7 +5943,7 @@
       </c>
       <c r="B38" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017232</t>
+          <t>SPBD241100017239</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
@@ -6092,7 +6092,7 @@
       </c>
       <c r="B39" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017235</t>
+          <t>SPBD241100017246</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
@@ -6241,7 +6241,7 @@
       </c>
       <c r="B40" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017239</t>
+          <t>SPBD241100017247</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -6390,7 +6390,7 @@
       </c>
       <c r="B41" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017246</t>
+          <t>SPBD241100017249</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
@@ -6539,7 +6539,7 @@
       </c>
       <c r="B42" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017247</t>
+          <t>SPBD241100017216</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -6688,7 +6688,7 @@
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017249</t>
+          <t>SPBD241100017223</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
@@ -6837,7 +6837,7 @@
       </c>
       <c r="B44" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017216</t>
+          <t>SPBD241100017230</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
@@ -6986,7 +6986,7 @@
       </c>
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017223</t>
+          <t>SPBD241100017238</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
@@ -7135,7 +7135,7 @@
       </c>
       <c r="B46" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017230</t>
+          <t>SPBD241100017240</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
@@ -7284,7 +7284,7 @@
       </c>
       <c r="B47" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017238</t>
+          <t>SPBD241100017220</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
@@ -7433,7 +7433,7 @@
       </c>
       <c r="B48" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017240</t>
+          <t>SPBD241100017221</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
@@ -7582,7 +7582,7 @@
       </c>
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017220</t>
+          <t>SPBD241100017227</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
@@ -7731,7 +7731,7 @@
       </c>
       <c r="B50" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017221</t>
+          <t>SPBD241100017229</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
@@ -7880,7 +7880,7 @@
       </c>
       <c r="B51" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017227</t>
+          <t>SPBD241100017234</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
@@ -8029,7 +8029,7 @@
       </c>
       <c r="B52" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017229</t>
+          <t>SPBD241100017241</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
@@ -8178,7 +8178,7 @@
       </c>
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017234</t>
+          <t>SPBD241100017244</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
@@ -8327,7 +8327,7 @@
       </c>
       <c r="B54" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017241</t>
+          <t>SPBD241100017252</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
@@ -8476,7 +8476,7 @@
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017244</t>
+          <t>SPBD241100017213</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
@@ -8625,7 +8625,7 @@
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017252</t>
+          <t>SPBD241100017214</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
@@ -8774,7 +8774,7 @@
       </c>
       <c r="B57" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017213</t>
+          <t>SPBD241100017231</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
@@ -8923,7 +8923,7 @@
       </c>
       <c r="B58" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017214</t>
+          <t>SPBD241100017243</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
@@ -9072,7 +9072,7 @@
       </c>
       <c r="B59" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017231</t>
+          <t>SPBD241100017250</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
@@ -9221,7 +9221,7 @@
       </c>
       <c r="B60" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017243</t>
+          <t>SPBD241100017251</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
@@ -9365,12 +9365,12 @@
     <row r="61" ht="13.2" customHeight="1" thickBot="1">
       <c r="A61" s="4" t="inlineStr">
         <is>
-          <t>21-11-2567</t>
+          <t>22-11-2567</t>
         </is>
       </c>
       <c r="B61" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017250</t>
+          <t>SPBD241100019897</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
@@ -9514,12 +9514,12 @@
     <row r="62" ht="13.2" customHeight="1" thickBot="1">
       <c r="A62" s="4" t="inlineStr">
         <is>
-          <t>21-11-2567</t>
+          <t>22-11-2567</t>
         </is>
       </c>
       <c r="B62" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100017251</t>
+          <t>SPBD241100019899</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr">
@@ -9668,7 +9668,7 @@
       </c>
       <c r="B63" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019897</t>
+          <t>SPBD241100019903</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
@@ -9817,7 +9817,7 @@
       </c>
       <c r="B64" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019899</t>
+          <t>SPBD241100019916</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
@@ -9966,7 +9966,7 @@
       </c>
       <c r="B65" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019903</t>
+          <t>SPBD241100019893</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
@@ -10115,7 +10115,7 @@
       </c>
       <c r="B66" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019916</t>
+          <t>SPBD241100019895</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
@@ -10264,7 +10264,7 @@
       </c>
       <c r="B67" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019893</t>
+          <t>SPBD241100019904</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
@@ -10413,7 +10413,7 @@
       </c>
       <c r="B68" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019895</t>
+          <t>SPBD241100019910</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
@@ -10562,7 +10562,7 @@
       </c>
       <c r="B69" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019904</t>
+          <t>SPBD241100019915</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
@@ -10711,7 +10711,7 @@
       </c>
       <c r="B70" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019910</t>
+          <t>SPBD241100019919</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
@@ -10860,7 +10860,7 @@
       </c>
       <c r="B71" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019915</t>
+          <t>SPBD241100019920</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
@@ -11009,7 +11009,7 @@
       </c>
       <c r="B72" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019919</t>
+          <t>SPBD241100019923</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
@@ -11158,7 +11158,7 @@
       </c>
       <c r="B73" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019920</t>
+          <t>SPBD241100019887</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
@@ -11307,7 +11307,7 @@
       </c>
       <c r="B74" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019923</t>
+          <t>SPBD241100019888</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
@@ -11456,7 +11456,7 @@
       </c>
       <c r="B75" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019887</t>
+          <t>SPBD241100019892</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
@@ -11605,7 +11605,7 @@
       </c>
       <c r="B76" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019888</t>
+          <t>SPBD241100019900</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
@@ -11754,7 +11754,7 @@
       </c>
       <c r="B77" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019892</t>
+          <t>SPBD241100019902</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
@@ -11903,7 +11903,7 @@
       </c>
       <c r="B78" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019900</t>
+          <t>SPBD241100019905</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
@@ -12052,7 +12052,7 @@
       </c>
       <c r="B79" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019902</t>
+          <t>SPBD241100019906</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
@@ -12201,7 +12201,7 @@
       </c>
       <c r="B80" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019905</t>
+          <t>SPBD241100019908</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
@@ -12350,7 +12350,7 @@
       </c>
       <c r="B81" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019906</t>
+          <t>SPBD241100019911</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
@@ -12499,7 +12499,7 @@
       </c>
       <c r="B82" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019908</t>
+          <t>SPBD241100019921</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
@@ -12648,7 +12648,7 @@
       </c>
       <c r="B83" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019911</t>
+          <t>SPBD241100019925</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
@@ -12797,7 +12797,7 @@
       </c>
       <c r="B84" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019921</t>
+          <t>SPBD241100019886</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
@@ -12946,7 +12946,7 @@
       </c>
       <c r="B85" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019925</t>
+          <t>SPBD241100019890</t>
         </is>
       </c>
       <c r="C85" s="3" t="inlineStr">
@@ -13095,7 +13095,7 @@
       </c>
       <c r="B86" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019886</t>
+          <t>SPBD241100019894</t>
         </is>
       </c>
       <c r="C86" s="3" t="inlineStr">
@@ -13244,7 +13244,7 @@
       </c>
       <c r="B87" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019890</t>
+          <t>SPBD241100019901</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
@@ -13393,7 +13393,7 @@
       </c>
       <c r="B88" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019894</t>
+          <t>SPBD241100019907</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
@@ -13542,7 +13542,7 @@
       </c>
       <c r="B89" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019901</t>
+          <t>SPBD241100019909</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
@@ -13691,7 +13691,7 @@
       </c>
       <c r="B90" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019907</t>
+          <t>SPBD241100019913</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
@@ -13840,7 +13840,7 @@
       </c>
       <c r="B91" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019909</t>
+          <t>SPBD241100019918</t>
         </is>
       </c>
       <c r="C91" s="3" t="inlineStr">
@@ -13989,7 +13989,7 @@
       </c>
       <c r="B92" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019913</t>
+          <t>SPBD241100019924</t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
@@ -14138,7 +14138,7 @@
       </c>
       <c r="B93" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019918</t>
+          <t>SPBD241100019891</t>
         </is>
       </c>
       <c r="C93" s="3" t="inlineStr">
@@ -14287,7 +14287,7 @@
       </c>
       <c r="B94" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019924</t>
+          <t>SPBD241100019912</t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
@@ -14436,7 +14436,7 @@
       </c>
       <c r="B95" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019891</t>
+          <t>SPBD241100019917</t>
         </is>
       </c>
       <c r="C95" s="3" t="inlineStr">
@@ -14585,7 +14585,7 @@
       </c>
       <c r="B96" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019912</t>
+          <t>SPBD241100019889</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
@@ -14734,7 +14734,7 @@
       </c>
       <c r="B97" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019917</t>
+          <t>SPBD241100019896</t>
         </is>
       </c>
       <c r="C97" s="3" t="inlineStr">
@@ -14883,7 +14883,7 @@
       </c>
       <c r="B98" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019889</t>
+          <t>SPBD241100019898</t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
@@ -15032,7 +15032,7 @@
       </c>
       <c r="B99" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019896</t>
+          <t>SPBD241100019914</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
@@ -15181,7 +15181,7 @@
       </c>
       <c r="B100" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019898</t>
+          <t>SPBD241100019922</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
@@ -15325,12 +15325,12 @@
     <row r="101" ht="13.2" customHeight="1" thickBot="1">
       <c r="A101" s="4" t="inlineStr">
         <is>
-          <t>22-11-2567</t>
+          <t>25-11-2567</t>
         </is>
       </c>
       <c r="B101" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019914</t>
+          <t>SPBD241100020298</t>
         </is>
       </c>
       <c r="C101" s="3" t="inlineStr">
@@ -15474,12 +15474,12 @@
     <row r="102" ht="13.2" customHeight="1" thickBot="1">
       <c r="A102" s="4" t="inlineStr">
         <is>
-          <t>22-11-2567</t>
+          <t>25-11-2567</t>
         </is>
       </c>
       <c r="B102" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100019922</t>
+          <t>SPBD241100020303</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
@@ -15628,7 +15628,7 @@
       </c>
       <c r="B103" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020298</t>
+          <t>SPBD241100020292</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
@@ -15777,7 +15777,7 @@
       </c>
       <c r="B104" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020303</t>
+          <t>SPBD241100020297</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
@@ -15926,7 +15926,7 @@
       </c>
       <c r="B105" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020292</t>
+          <t>SPBD241100020299</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
@@ -16075,7 +16075,7 @@
       </c>
       <c r="B106" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020297</t>
+          <t>SPBD241100020302</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
@@ -16224,7 +16224,7 @@
       </c>
       <c r="B107" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020299</t>
+          <t>SPBD241100020304</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
@@ -16373,7 +16373,7 @@
       </c>
       <c r="B108" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020302</t>
+          <t>SPBD241100020309</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
@@ -16522,7 +16522,7 @@
       </c>
       <c r="B109" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020304</t>
+          <t>SPBD241100020278</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
@@ -16671,7 +16671,7 @@
       </c>
       <c r="B110" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020309</t>
+          <t>SPBD241100020280</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
@@ -16820,7 +16820,7 @@
       </c>
       <c r="B111" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020278</t>
+          <t>SPBD241100020286</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
@@ -16969,7 +16969,7 @@
       </c>
       <c r="B112" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020280</t>
+          <t>SPBD241100020294</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
@@ -17118,7 +17118,7 @@
       </c>
       <c r="B113" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020286</t>
+          <t>SPBD241100020301</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
@@ -17267,7 +17267,7 @@
       </c>
       <c r="B114" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020294</t>
+          <t>SPBD241100020310</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
@@ -17416,7 +17416,7 @@
       </c>
       <c r="B115" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020301</t>
+          <t>SPBD241100020311</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
@@ -17565,7 +17565,7 @@
       </c>
       <c r="B116" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020310</t>
+          <t>SPBD241100020276</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
@@ -17714,7 +17714,7 @@
       </c>
       <c r="B117" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020311</t>
+          <t>SPBD241100020285</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
@@ -17863,7 +17863,7 @@
       </c>
       <c r="B118" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020276</t>
+          <t>SPBD241100020288</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
@@ -18012,7 +18012,7 @@
       </c>
       <c r="B119" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020285</t>
+          <t>SPBD241100020290</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
@@ -18161,7 +18161,7 @@
       </c>
       <c r="B120" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020288</t>
+          <t>SPBD241100020308</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
@@ -18310,7 +18310,7 @@
       </c>
       <c r="B121" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020290</t>
+          <t>SPBD241100020312</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
@@ -18459,7 +18459,7 @@
       </c>
       <c r="B122" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020308</t>
+          <t>SPBD241100020313</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
@@ -18608,7 +18608,7 @@
       </c>
       <c r="B123" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020312</t>
+          <t>SPBD241100020314</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
@@ -18757,7 +18757,7 @@
       </c>
       <c r="B124" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020313</t>
+          <t>SPBD241100020315</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
@@ -18906,7 +18906,7 @@
       </c>
       <c r="B125" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020314</t>
+          <t>SPBD241100020277</t>
         </is>
       </c>
       <c r="C125" s="3" t="inlineStr">
@@ -19055,7 +19055,7 @@
       </c>
       <c r="B126" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020315</t>
+          <t>SPBD241100020281</t>
         </is>
       </c>
       <c r="C126" s="3" t="inlineStr">
@@ -19204,7 +19204,7 @@
       </c>
       <c r="B127" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020277</t>
+          <t>SPBD241100020284</t>
         </is>
       </c>
       <c r="C127" s="3" t="inlineStr">
@@ -19353,7 +19353,7 @@
       </c>
       <c r="B128" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020281</t>
+          <t>SPBD241100020287</t>
         </is>
       </c>
       <c r="C128" s="3" t="inlineStr">
@@ -19502,7 +19502,7 @@
       </c>
       <c r="B129" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020284</t>
+          <t>SPBD241100020291</t>
         </is>
       </c>
       <c r="C129" s="3" t="inlineStr">
@@ -19651,7 +19651,7 @@
       </c>
       <c r="B130" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020287</t>
+          <t>SPBD241100020296</t>
         </is>
       </c>
       <c r="C130" s="3" t="inlineStr">
@@ -19800,7 +19800,7 @@
       </c>
       <c r="B131" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020291</t>
+          <t>SPBD241100020279</t>
         </is>
       </c>
       <c r="C131" s="3" t="inlineStr">
@@ -19949,7 +19949,7 @@
       </c>
       <c r="B132" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020296</t>
+          <t>SPBD241100020282</t>
         </is>
       </c>
       <c r="C132" s="3" t="inlineStr">
@@ -20098,7 +20098,7 @@
       </c>
       <c r="B133" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020279</t>
+          <t>SPBD241100020283</t>
         </is>
       </c>
       <c r="C133" s="3" t="inlineStr">
@@ -20247,7 +20247,7 @@
       </c>
       <c r="B134" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020282</t>
+          <t>SPBD241100020289</t>
         </is>
       </c>
       <c r="C134" s="3" t="inlineStr">
@@ -20396,7 +20396,7 @@
       </c>
       <c r="B135" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020283</t>
+          <t>SPBD241100020293</t>
         </is>
       </c>
       <c r="C135" s="3" t="inlineStr">
@@ -20545,7 +20545,7 @@
       </c>
       <c r="B136" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020289</t>
+          <t>SPBD241100020295</t>
         </is>
       </c>
       <c r="C136" s="3" t="inlineStr">
@@ -20694,7 +20694,7 @@
       </c>
       <c r="B137" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020293</t>
+          <t>SPBD241100020300</t>
         </is>
       </c>
       <c r="C137" s="3" t="inlineStr">
@@ -20843,7 +20843,7 @@
       </c>
       <c r="B138" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020295</t>
+          <t>SPBD241100020305</t>
         </is>
       </c>
       <c r="C138" s="3" t="inlineStr">
@@ -20992,7 +20992,7 @@
       </c>
       <c r="B139" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020300</t>
+          <t>SPBD241100020306</t>
         </is>
       </c>
       <c r="C139" s="3" t="inlineStr">
@@ -21141,7 +21141,7 @@
       </c>
       <c r="B140" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020305</t>
+          <t>SPBD241100020307</t>
         </is>
       </c>
       <c r="C140" s="3" t="inlineStr">
@@ -21285,12 +21285,12 @@
     <row r="141" ht="13.2" customHeight="1" thickBot="1">
       <c r="A141" s="4" t="inlineStr">
         <is>
-          <t>25-11-2567</t>
+          <t>26-11-2567</t>
         </is>
       </c>
       <c r="B141" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020306</t>
+          <t>SPBD241100021257</t>
         </is>
       </c>
       <c r="C141" s="3" t="inlineStr">
@@ -21434,12 +21434,12 @@
     <row r="142" ht="13.2" customHeight="1" thickBot="1">
       <c r="A142" s="4" t="inlineStr">
         <is>
-          <t>25-11-2567</t>
+          <t>26-11-2567</t>
         </is>
       </c>
       <c r="B142" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100020307</t>
+          <t>SPBD241100021258</t>
         </is>
       </c>
       <c r="C142" s="3" t="inlineStr">
@@ -21588,7 +21588,7 @@
       </c>
       <c r="B143" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021257</t>
+          <t>SPBD241100021262</t>
         </is>
       </c>
       <c r="C143" s="3" t="inlineStr">
@@ -21737,7 +21737,7 @@
       </c>
       <c r="B144" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021258</t>
+          <t>SPBD241100021267</t>
         </is>
       </c>
       <c r="C144" s="3" t="inlineStr">
@@ -21886,7 +21886,7 @@
       </c>
       <c r="B145" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021262</t>
+          <t>SPBD241100021280</t>
         </is>
       </c>
       <c r="C145" s="3" t="inlineStr">
@@ -22035,7 +22035,7 @@
       </c>
       <c r="B146" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021267</t>
+          <t>SPBD241100021287</t>
         </is>
       </c>
       <c r="C146" s="3" t="inlineStr">
@@ -22184,7 +22184,7 @@
       </c>
       <c r="B147" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021280</t>
+          <t>SPBD241100021289</t>
         </is>
       </c>
       <c r="C147" s="3" t="inlineStr">
@@ -22333,7 +22333,7 @@
       </c>
       <c r="B148" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021287</t>
+          <t>SPBD241100021260</t>
         </is>
       </c>
       <c r="C148" s="3" t="inlineStr">
@@ -22482,7 +22482,7 @@
       </c>
       <c r="B149" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021289</t>
+          <t>SPBD241100021261</t>
         </is>
       </c>
       <c r="C149" s="3" t="inlineStr">
@@ -22631,7 +22631,7 @@
       </c>
       <c r="B150" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021260</t>
+          <t>SPBD241100021265</t>
         </is>
       </c>
       <c r="C150" s="3" t="inlineStr">
@@ -22780,7 +22780,7 @@
       </c>
       <c r="B151" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021261</t>
+          <t>SPBD241100021270</t>
         </is>
       </c>
       <c r="C151" s="3" t="inlineStr">
@@ -22929,7 +22929,7 @@
       </c>
       <c r="B152" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021265</t>
+          <t>SPBD241100021272</t>
         </is>
       </c>
       <c r="C152" s="3" t="inlineStr">
@@ -23078,7 +23078,7 @@
       </c>
       <c r="B153" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021270</t>
+          <t>SPBD241100021273</t>
         </is>
       </c>
       <c r="C153" s="3" t="inlineStr">
@@ -23227,7 +23227,7 @@
       </c>
       <c r="B154" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021272</t>
+          <t>SPBD241100021278</t>
         </is>
       </c>
       <c r="C154" s="3" t="inlineStr">
@@ -23376,7 +23376,7 @@
       </c>
       <c r="B155" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021273</t>
+          <t>SPBD241100021282</t>
         </is>
       </c>
       <c r="C155" s="3" t="inlineStr">
@@ -23525,7 +23525,7 @@
       </c>
       <c r="B156" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021278</t>
+          <t>SPBD241100021290</t>
         </is>
       </c>
       <c r="C156" s="3" t="inlineStr">
@@ -23674,7 +23674,7 @@
       </c>
       <c r="B157" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021282</t>
+          <t>SPBD241100021291</t>
         </is>
       </c>
       <c r="C157" s="3" t="inlineStr">
@@ -23823,7 +23823,7 @@
       </c>
       <c r="B158" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021290</t>
+          <t>SPBD241100021253</t>
         </is>
       </c>
       <c r="C158" s="3" t="inlineStr">
@@ -23972,7 +23972,7 @@
       </c>
       <c r="B159" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021291</t>
+          <t>SPBD241100021274</t>
         </is>
       </c>
       <c r="C159" s="3" t="inlineStr">
@@ -24121,7 +24121,7 @@
       </c>
       <c r="B160" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021253</t>
+          <t>SPBD241100021276</t>
         </is>
       </c>
       <c r="C160" s="3" t="inlineStr">
@@ -24270,7 +24270,7 @@
       </c>
       <c r="B161" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021274</t>
+          <t>SPBD241100021277</t>
         </is>
       </c>
       <c r="C161" s="3" t="inlineStr">
@@ -24419,7 +24419,7 @@
       </c>
       <c r="B162" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021276</t>
+          <t>SPBD241100021283</t>
         </is>
       </c>
       <c r="C162" s="3" t="inlineStr">
@@ -24568,7 +24568,7 @@
       </c>
       <c r="B163" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021277</t>
+          <t>SPBD241100021285</t>
         </is>
       </c>
       <c r="C163" s="3" t="inlineStr">
@@ -24717,7 +24717,7 @@
       </c>
       <c r="B164" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021283</t>
+          <t>SPBD241100021286</t>
         </is>
       </c>
       <c r="C164" s="3" t="inlineStr">
@@ -24866,7 +24866,7 @@
       </c>
       <c r="B165" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021285</t>
+          <t>SPBD241100021288</t>
         </is>
       </c>
       <c r="C165" s="3" t="inlineStr">
@@ -25015,7 +25015,7 @@
       </c>
       <c r="B166" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021286</t>
+          <t>SPBD241100021255</t>
         </is>
       </c>
       <c r="C166" s="3" t="inlineStr">
@@ -25164,7 +25164,7 @@
       </c>
       <c r="B167" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021288</t>
+          <t>SPBD241100021264</t>
         </is>
       </c>
       <c r="C167" s="3" t="inlineStr">
@@ -25313,7 +25313,7 @@
       </c>
       <c r="B168" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021255</t>
+          <t>SPBD241100021266</t>
         </is>
       </c>
       <c r="C168" s="3" t="inlineStr">
@@ -25462,7 +25462,7 @@
       </c>
       <c r="B169" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021264</t>
+          <t>SPBD241100021269</t>
         </is>
       </c>
       <c r="C169" s="3" t="inlineStr">
@@ -25611,7 +25611,7 @@
       </c>
       <c r="B170" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021266</t>
+          <t>SPBD241100021279</t>
         </is>
       </c>
       <c r="C170" s="3" t="inlineStr">
@@ -25760,7 +25760,7 @@
       </c>
       <c r="B171" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021269</t>
+          <t>SPBD241100021281</t>
         </is>
       </c>
       <c r="C171" s="3" t="inlineStr">
@@ -25909,7 +25909,7 @@
       </c>
       <c r="B172" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021279</t>
+          <t>SPBD241100021252</t>
         </is>
       </c>
       <c r="C172" s="3" t="inlineStr">
@@ -26058,7 +26058,7 @@
       </c>
       <c r="B173" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021281</t>
+          <t>SPBD241100021254</t>
         </is>
       </c>
       <c r="C173" s="3" t="inlineStr">
@@ -26207,7 +26207,7 @@
       </c>
       <c r="B174" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021252</t>
+          <t>SPBD241100021263</t>
         </is>
       </c>
       <c r="C174" s="3" t="inlineStr">
@@ -26356,7 +26356,7 @@
       </c>
       <c r="B175" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021254</t>
+          <t>SPBD241100021275</t>
         </is>
       </c>
       <c r="C175" s="3" t="inlineStr">
@@ -26505,7 +26505,7 @@
       </c>
       <c r="B176" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021263</t>
+          <t>SPBD241100021256</t>
         </is>
       </c>
       <c r="C176" s="3" t="inlineStr">
@@ -26654,7 +26654,7 @@
       </c>
       <c r="B177" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021275</t>
+          <t>SPBD241100021259</t>
         </is>
       </c>
       <c r="C177" s="3" t="inlineStr">
@@ -26803,7 +26803,7 @@
       </c>
       <c r="B178" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021256</t>
+          <t>SPBD241100021268</t>
         </is>
       </c>
       <c r="C178" s="3" t="inlineStr">
@@ -26952,7 +26952,7 @@
       </c>
       <c r="B179" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021259</t>
+          <t>SPBD241100021271</t>
         </is>
       </c>
       <c r="C179" s="3" t="inlineStr">
@@ -27101,7 +27101,7 @@
       </c>
       <c r="B180" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021268</t>
+          <t>SPBD241100021284</t>
         </is>
       </c>
       <c r="C180" s="3" t="inlineStr">
@@ -27245,12 +27245,12 @@
     <row r="181" ht="13.2" customHeight="1" thickBot="1">
       <c r="A181" s="4" t="inlineStr">
         <is>
-          <t>26-11-2567</t>
+          <t>27-11-2567</t>
         </is>
       </c>
       <c r="B181" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021271</t>
+          <t>SPBD241100021782</t>
         </is>
       </c>
       <c r="C181" s="3" t="inlineStr">
@@ -27394,12 +27394,12 @@
     <row r="182" ht="13.2" customHeight="1" thickBot="1">
       <c r="A182" s="4" t="inlineStr">
         <is>
-          <t>26-11-2567</t>
+          <t>27-11-2567</t>
         </is>
       </c>
       <c r="B182" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021284</t>
+          <t>SPBD241100021784</t>
         </is>
       </c>
       <c r="C182" s="3" t="inlineStr">
@@ -27548,7 +27548,7 @@
       </c>
       <c r="B183" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021782</t>
+          <t>SPBD241100021809</t>
         </is>
       </c>
       <c r="C183" s="3" t="inlineStr">
@@ -27697,7 +27697,7 @@
       </c>
       <c r="B184" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021784</t>
+          <t>SPBD241100021814</t>
         </is>
       </c>
       <c r="C184" s="3" t="inlineStr">
@@ -27846,7 +27846,7 @@
       </c>
       <c r="B185" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021809</t>
+          <t>SPBD241100021786</t>
         </is>
       </c>
       <c r="C185" s="3" t="inlineStr">
@@ -27995,7 +27995,7 @@
       </c>
       <c r="B186" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021814</t>
+          <t>SPBD241100021787</t>
         </is>
       </c>
       <c r="C186" s="3" t="inlineStr">
@@ -28144,7 +28144,7 @@
       </c>
       <c r="B187" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021786</t>
+          <t>SPBD241100021791</t>
         </is>
       </c>
       <c r="C187" s="3" t="inlineStr">
@@ -28293,7 +28293,7 @@
       </c>
       <c r="B188" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021787</t>
+          <t>SPBD241100021793</t>
         </is>
       </c>
       <c r="C188" s="3" t="inlineStr">
@@ -28442,7 +28442,7 @@
       </c>
       <c r="B189" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021791</t>
+          <t>SPBD241100021796</t>
         </is>
       </c>
       <c r="C189" s="3" t="inlineStr">
@@ -28591,7 +28591,7 @@
       </c>
       <c r="B190" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021793</t>
+          <t>SPBD241100021797</t>
         </is>
       </c>
       <c r="C190" s="3" t="inlineStr">
@@ -28740,7 +28740,7 @@
       </c>
       <c r="B191" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021796</t>
+          <t>SPBD241100021800</t>
         </is>
       </c>
       <c r="C191" s="3" t="inlineStr">
@@ -28889,7 +28889,7 @@
       </c>
       <c r="B192" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021797</t>
+          <t>SPBD241100021802</t>
         </is>
       </c>
       <c r="C192" s="3" t="inlineStr">
@@ -29038,7 +29038,7 @@
       </c>
       <c r="B193" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021800</t>
+          <t>SPBD241100021806</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
@@ -29187,7 +29187,7 @@
       </c>
       <c r="B194" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021802</t>
+          <t>SPBD241100021808</t>
         </is>
       </c>
       <c r="C194" s="3" t="inlineStr">
@@ -29336,7 +29336,7 @@
       </c>
       <c r="B195" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021806</t>
+          <t>SPBD241100021810</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
@@ -29485,7 +29485,7 @@
       </c>
       <c r="B196" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021808</t>
+          <t>SPBD241100021813</t>
         </is>
       </c>
       <c r="C196" s="3" t="inlineStr">
@@ -29634,7 +29634,7 @@
       </c>
       <c r="B197" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021810</t>
+          <t>SPBD241100021816</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
@@ -29783,7 +29783,7 @@
       </c>
       <c r="B198" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021813</t>
+          <t>SPBD241100021788</t>
         </is>
       </c>
       <c r="C198" s="3" t="inlineStr">
@@ -29932,7 +29932,7 @@
       </c>
       <c r="B199" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021816</t>
+          <t>SPBD241100021789</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
@@ -30081,7 +30081,7 @@
       </c>
       <c r="B200" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021788</t>
+          <t>SPBD241100021790</t>
         </is>
       </c>
       <c r="C200" s="3" t="inlineStr">
@@ -30230,7 +30230,7 @@
       </c>
       <c r="B201" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021789</t>
+          <t>SPBD241100021795</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
@@ -30379,7 +30379,7 @@
       </c>
       <c r="B202" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021790</t>
+          <t>SPBD241100021805</t>
         </is>
       </c>
       <c r="C202" s="3" t="inlineStr">
@@ -30528,7 +30528,7 @@
       </c>
       <c r="B203" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021795</t>
+          <t>SPBD241100021817</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
@@ -30677,7 +30677,7 @@
       </c>
       <c r="B204" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021805</t>
+          <t>SPBD241100021783</t>
         </is>
       </c>
       <c r="C204" s="3" t="inlineStr">
@@ -30826,7 +30826,7 @@
       </c>
       <c r="B205" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021817</t>
+          <t>SPBD241100021785</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
@@ -30975,7 +30975,7 @@
       </c>
       <c r="B206" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021783</t>
+          <t>SPBD241100021799</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
@@ -31124,7 +31124,7 @@
       </c>
       <c r="B207" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021785</t>
+          <t>SPBD241100021801</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
@@ -31273,7 +31273,7 @@
       </c>
       <c r="B208" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021799</t>
+          <t>SPBD241100021803</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
@@ -31422,7 +31422,7 @@
       </c>
       <c r="B209" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021801</t>
+          <t>SPBD241100021804</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
@@ -31571,7 +31571,7 @@
       </c>
       <c r="B210" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021803</t>
+          <t>SPBD241100021812</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
@@ -31720,7 +31720,7 @@
       </c>
       <c r="B211" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021804</t>
+          <t>SPBD241100021781</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
@@ -31869,7 +31869,7 @@
       </c>
       <c r="B212" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021812</t>
+          <t>SPBD241100021792</t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
@@ -32018,7 +32018,7 @@
       </c>
       <c r="B213" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021781</t>
+          <t>SPBD241100021794</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
@@ -32167,7 +32167,7 @@
       </c>
       <c r="B214" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021792</t>
+          <t>SPBD241100021807</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
@@ -32316,7 +32316,7 @@
       </c>
       <c r="B215" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021794</t>
+          <t>SPBD241100021815</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
@@ -32465,7 +32465,7 @@
       </c>
       <c r="B216" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021807</t>
+          <t>SPBD241100021818</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
@@ -32614,7 +32614,7 @@
       </c>
       <c r="B217" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021815</t>
+          <t>SPBD241100021780</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
@@ -32763,7 +32763,7 @@
       </c>
       <c r="B218" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021818</t>
+          <t>SPBD241100021798</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
@@ -32912,7 +32912,7 @@
       </c>
       <c r="B219" s="4" t="inlineStr">
         <is>
-          <t>SPBD241100021780</t>
+          <t>SPBD241100021811</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
@@ -33054,131 +33054,31 @@
       <c r="AU219" s="3" t="n"/>
     </row>
     <row r="220" ht="13.2" customHeight="1" thickBot="1">
-      <c r="A220" s="4" t="inlineStr">
-        <is>
-          <t>27-11-2567</t>
-        </is>
-      </c>
-      <c r="B220" s="4" t="inlineStr">
-        <is>
-          <t>SPBD241100021798</t>
-        </is>
-      </c>
-      <c r="C220" s="3" t="inlineStr">
-        <is>
-          <t>0002400563</t>
-        </is>
-      </c>
-      <c r="D220" s="3" t="inlineStr">
-        <is>
-          <t>120 ซม.</t>
-        </is>
-      </c>
-      <c r="E220" s="3" t="inlineStr">
-        <is>
-          <t>กล่อง L</t>
-        </is>
-      </c>
-      <c r="F220" s="3" t="inlineStr">
-        <is>
-          <t>Flash</t>
-        </is>
-      </c>
-      <c r="G220" s="3" t="inlineStr">
-        <is>
-          <t>DCBB</t>
-        </is>
-      </c>
-      <c r="H220" s="3" t="inlineStr">
-        <is>
-          <t>Home (11120)</t>
-        </is>
-      </c>
-      <c r="I220" s="3" t="inlineStr">
-        <is>
-          <t>คุณ a</t>
-        </is>
-      </c>
-      <c r="J220" s="3" t="inlineStr">
-        <is>
-          <t>0633906216</t>
-        </is>
-      </c>
-      <c r="K220" s="3" t="inlineStr">
-        <is>
-          <t>สาขา คุณาลัย-บางใหญ่ (07465)</t>
-        </is>
-      </c>
-      <c r="L220" s="3" t="inlineStr">
-        <is>
-          <t>74 ลำพยา เมืองนครปฐม นครปฐม 73000</t>
-        </is>
-      </c>
-      <c r="M220" s="3" t="inlineStr">
-        <is>
-          <t>ทดสอบพัสดุCourier</t>
-        </is>
-      </c>
-      <c r="N220" s="3" t="inlineStr">
-        <is>
-          <t>0971971445</t>
-        </is>
-      </c>
-      <c r="O220" s="3" t="inlineStr">
-        <is>
-          <t>บ้าน</t>
-        </is>
-      </c>
-      <c r="P220" s="3" t="inlineStr">
-        <is>
-          <t>554 หมู่ 3 ปากเกร็ด ปากเกร็ด นนทบุรี 11120</t>
-        </is>
-      </c>
-      <c r="Q220" s="3" t="inlineStr">
-        <is>
-          <t>73000</t>
-        </is>
-      </c>
-      <c r="R220" s="3" t="inlineStr">
-        <is>
-          <t>11120</t>
-        </is>
-      </c>
-      <c r="S220" s="3" t="inlineStr">
-        <is>
-          <t>Non COD</t>
-        </is>
-      </c>
-      <c r="T220" s="3" t="inlineStr">
-        <is>
-          <t>ไม่มีการซื้อประกัน</t>
-        </is>
-      </c>
-      <c r="U220" s="3" t="inlineStr">
-        <is>
-          <t>FSH</t>
-        </is>
-      </c>
-      <c r="V220" s="3" t="inlineStr">
-        <is>
-          <t>11120 (กล่อง L)</t>
-        </is>
-      </c>
-      <c r="W220" s="3" t="inlineStr">
-        <is>
-          <t>นนทบุรี</t>
-        </is>
-      </c>
-      <c r="X220" s="3" t="inlineStr">
-        <is>
-          <t>ทดสอบพัสดุCourier</t>
-        </is>
-      </c>
-      <c r="Y220" s="3" t="inlineStr">
-        <is>
-          <t>0971971445</t>
-        </is>
-      </c>
+      <c r="A220" s="3" t="n"/>
+      <c r="B220" s="3" t="n"/>
+      <c r="C220" s="3" t="n"/>
+      <c r="D220" s="3" t="n"/>
+      <c r="E220" s="3" t="n"/>
+      <c r="F220" s="3" t="n"/>
+      <c r="G220" s="3" t="n"/>
+      <c r="H220" s="3" t="n"/>
+      <c r="I220" s="3" t="n"/>
+      <c r="J220" s="3" t="n"/>
+      <c r="K220" s="3" t="n"/>
+      <c r="L220" s="3" t="n"/>
+      <c r="M220" s="3" t="n"/>
+      <c r="N220" s="3" t="n"/>
+      <c r="O220" s="3" t="n"/>
+      <c r="P220" s="3" t="n"/>
+      <c r="Q220" s="3" t="n"/>
+      <c r="R220" s="3" t="n"/>
+      <c r="S220" s="3" t="n"/>
+      <c r="T220" s="3" t="n"/>
+      <c r="U220" s="3" t="n"/>
+      <c r="V220" s="3" t="n"/>
+      <c r="W220" s="3" t="n"/>
+      <c r="X220" s="3" t="n"/>
+      <c r="Y220" s="3" t="n"/>
       <c r="Z220" s="3" t="n"/>
       <c r="AA220" s="3" t="n"/>
       <c r="AB220" s="3" t="n"/>
@@ -33203,131 +33103,31 @@
       <c r="AU220" s="3" t="n"/>
     </row>
     <row r="221" ht="13.2" customHeight="1" thickBot="1">
-      <c r="A221" s="4" t="inlineStr">
-        <is>
-          <t>27-11-2567</t>
-        </is>
-      </c>
-      <c r="B221" s="4" t="inlineStr">
-        <is>
-          <t>SPBD241100021811</t>
-        </is>
-      </c>
-      <c r="C221" s="3" t="inlineStr">
-        <is>
-          <t>0002400563</t>
-        </is>
-      </c>
-      <c r="D221" s="3" t="inlineStr">
-        <is>
-          <t>120 ซม.</t>
-        </is>
-      </c>
-      <c r="E221" s="3" t="inlineStr">
-        <is>
-          <t>กล่อง L</t>
-        </is>
-      </c>
-      <c r="F221" s="3" t="inlineStr">
-        <is>
-          <t>Flash</t>
-        </is>
-      </c>
-      <c r="G221" s="3" t="inlineStr">
-        <is>
-          <t>DCBB</t>
-        </is>
-      </c>
-      <c r="H221" s="3" t="inlineStr">
-        <is>
-          <t>Home (11120)</t>
-        </is>
-      </c>
-      <c r="I221" s="3" t="inlineStr">
-        <is>
-          <t>คุณ a</t>
-        </is>
-      </c>
-      <c r="J221" s="3" t="inlineStr">
-        <is>
-          <t>0633906216</t>
-        </is>
-      </c>
-      <c r="K221" s="3" t="inlineStr">
-        <is>
-          <t>สาขา คุณาลัย-บางใหญ่ (07465)</t>
-        </is>
-      </c>
-      <c r="L221" s="3" t="inlineStr">
-        <is>
-          <t>74 ลำพยา เมืองนครปฐม นครปฐม 73000</t>
-        </is>
-      </c>
-      <c r="M221" s="3" t="inlineStr">
-        <is>
-          <t>ทดสอบพัสดุCourier</t>
-        </is>
-      </c>
-      <c r="N221" s="3" t="inlineStr">
-        <is>
-          <t>0971971445</t>
-        </is>
-      </c>
-      <c r="O221" s="3" t="inlineStr">
-        <is>
-          <t>บ้าน</t>
-        </is>
-      </c>
-      <c r="P221" s="3" t="inlineStr">
-        <is>
-          <t>554 หมู่ 3 ปากเกร็ด ปากเกร็ด นนทบุรี 11120</t>
-        </is>
-      </c>
-      <c r="Q221" s="3" t="inlineStr">
-        <is>
-          <t>73000</t>
-        </is>
-      </c>
-      <c r="R221" s="3" t="inlineStr">
-        <is>
-          <t>11120</t>
-        </is>
-      </c>
-      <c r="S221" s="3" t="inlineStr">
-        <is>
-          <t>Non COD</t>
-        </is>
-      </c>
-      <c r="T221" s="3" t="inlineStr">
-        <is>
-          <t>ไม่มีการซื้อประกัน</t>
-        </is>
-      </c>
-      <c r="U221" s="3" t="inlineStr">
-        <is>
-          <t>FSH</t>
-        </is>
-      </c>
-      <c r="V221" s="3" t="inlineStr">
-        <is>
-          <t>11120 (กล่อง L)</t>
-        </is>
-      </c>
-      <c r="W221" s="3" t="inlineStr">
-        <is>
-          <t>นนทบุรี</t>
-        </is>
-      </c>
-      <c r="X221" s="3" t="inlineStr">
-        <is>
-          <t>ทดสอบพัสดุCourier</t>
-        </is>
-      </c>
-      <c r="Y221" s="3" t="inlineStr">
-        <is>
-          <t>0971971445</t>
-        </is>
-      </c>
+      <c r="A221" s="3" t="n"/>
+      <c r="B221" s="3" t="n"/>
+      <c r="C221" s="3" t="n"/>
+      <c r="D221" s="3" t="n"/>
+      <c r="E221" s="3" t="n"/>
+      <c r="F221" s="3" t="n"/>
+      <c r="G221" s="3" t="n"/>
+      <c r="H221" s="3" t="n"/>
+      <c r="I221" s="3" t="n"/>
+      <c r="J221" s="3" t="n"/>
+      <c r="K221" s="3" t="n"/>
+      <c r="L221" s="3" t="n"/>
+      <c r="M221" s="3" t="n"/>
+      <c r="N221" s="3" t="n"/>
+      <c r="O221" s="3" t="n"/>
+      <c r="P221" s="3" t="n"/>
+      <c r="Q221" s="3" t="n"/>
+      <c r="R221" s="3" t="n"/>
+      <c r="S221" s="3" t="n"/>
+      <c r="T221" s="3" t="n"/>
+      <c r="U221" s="3" t="n"/>
+      <c r="V221" s="3" t="n"/>
+      <c r="W221" s="3" t="n"/>
+      <c r="X221" s="3" t="n"/>
+      <c r="Y221" s="3" t="n"/>
       <c r="Z221" s="3" t="n"/>
       <c r="AA221" s="3" t="n"/>
       <c r="AB221" s="3" t="n"/>
@@ -48296,104 +48096,8 @@
       <c r="AT526" s="3" t="n"/>
       <c r="AU526" s="3" t="n"/>
     </row>
-    <row r="527" ht="13.2" customHeight="1">
-      <c r="A527" s="3" t="n"/>
-      <c r="B527" s="3" t="n"/>
-      <c r="C527" s="3" t="n"/>
-      <c r="D527" s="3" t="n"/>
-      <c r="E527" s="3" t="n"/>
-      <c r="F527" s="3" t="n"/>
-      <c r="G527" s="3" t="n"/>
-      <c r="H527" s="3" t="n"/>
-      <c r="I527" s="3" t="n"/>
-      <c r="J527" s="3" t="n"/>
-      <c r="K527" s="3" t="n"/>
-      <c r="L527" s="3" t="n"/>
-      <c r="M527" s="3" t="n"/>
-      <c r="N527" s="3" t="n"/>
-      <c r="O527" s="3" t="n"/>
-      <c r="P527" s="3" t="n"/>
-      <c r="Q527" s="3" t="n"/>
-      <c r="R527" s="3" t="n"/>
-      <c r="S527" s="3" t="n"/>
-      <c r="T527" s="3" t="n"/>
-      <c r="U527" s="3" t="n"/>
-      <c r="V527" s="3" t="n"/>
-      <c r="W527" s="3" t="n"/>
-      <c r="X527" s="3" t="n"/>
-      <c r="Y527" s="3" t="n"/>
-      <c r="Z527" s="3" t="n"/>
-      <c r="AA527" s="3" t="n"/>
-      <c r="AB527" s="3" t="n"/>
-      <c r="AC527" s="3" t="n"/>
-      <c r="AD527" s="3" t="n"/>
-      <c r="AE527" s="3" t="n"/>
-      <c r="AF527" s="3" t="n"/>
-      <c r="AG527" s="3" t="n"/>
-      <c r="AH527" s="3" t="n"/>
-      <c r="AI527" s="3" t="n"/>
-      <c r="AJ527" s="3" t="n"/>
-      <c r="AK527" s="3" t="n"/>
-      <c r="AL527" s="3" t="n"/>
-      <c r="AM527" s="3" t="n"/>
-      <c r="AN527" s="3" t="n"/>
-      <c r="AO527" s="3" t="n"/>
-      <c r="AP527" s="3" t="n"/>
-      <c r="AQ527" s="3" t="n"/>
-      <c r="AR527" s="3" t="n"/>
-      <c r="AS527" s="3" t="n"/>
-      <c r="AT527" s="3" t="n"/>
-      <c r="AU527" s="3" t="n"/>
-    </row>
-    <row r="528" ht="13.2" customHeight="1">
-      <c r="A528" s="3" t="n"/>
-      <c r="B528" s="3" t="n"/>
-      <c r="C528" s="3" t="n"/>
-      <c r="D528" s="3" t="n"/>
-      <c r="E528" s="3" t="n"/>
-      <c r="F528" s="3" t="n"/>
-      <c r="G528" s="3" t="n"/>
-      <c r="H528" s="3" t="n"/>
-      <c r="I528" s="3" t="n"/>
-      <c r="J528" s="3" t="n"/>
-      <c r="K528" s="3" t="n"/>
-      <c r="L528" s="3" t="n"/>
-      <c r="M528" s="3" t="n"/>
-      <c r="N528" s="3" t="n"/>
-      <c r="O528" s="3" t="n"/>
-      <c r="P528" s="3" t="n"/>
-      <c r="Q528" s="3" t="n"/>
-      <c r="R528" s="3" t="n"/>
-      <c r="S528" s="3" t="n"/>
-      <c r="T528" s="3" t="n"/>
-      <c r="U528" s="3" t="n"/>
-      <c r="V528" s="3" t="n"/>
-      <c r="W528" s="3" t="n"/>
-      <c r="X528" s="3" t="n"/>
-      <c r="Y528" s="3" t="n"/>
-      <c r="Z528" s="3" t="n"/>
-      <c r="AA528" s="3" t="n"/>
-      <c r="AB528" s="3" t="n"/>
-      <c r="AC528" s="3" t="n"/>
-      <c r="AD528" s="3" t="n"/>
-      <c r="AE528" s="3" t="n"/>
-      <c r="AF528" s="3" t="n"/>
-      <c r="AG528" s="3" t="n"/>
-      <c r="AH528" s="3" t="n"/>
-      <c r="AI528" s="3" t="n"/>
-      <c r="AJ528" s="3" t="n"/>
-      <c r="AK528" s="3" t="n"/>
-      <c r="AL528" s="3" t="n"/>
-      <c r="AM528" s="3" t="n"/>
-      <c r="AN528" s="3" t="n"/>
-      <c r="AO528" s="3" t="n"/>
-      <c r="AP528" s="3" t="n"/>
-      <c r="AQ528" s="3" t="n"/>
-      <c r="AR528" s="3" t="n"/>
-      <c r="AS528" s="3" t="n"/>
-      <c r="AT528" s="3" t="n"/>
-      <c r="AU528" s="3" t="n"/>
-    </row>
+    <row r="527" ht="13.2" customHeight="1"/>
+    <row r="528" ht="13.2" customHeight="1"/>
     <row r="529" ht="13.2" customHeight="1"/>
     <row r="530" ht="13.2" customHeight="1"/>
     <row r="531" ht="13.2" customHeight="1"/>

</xml_diff>